<commit_message>
added 2017 ranking data
</commit_message>
<xml_diff>
--- a/Data/EmploymentSummary-2017.xlsx
+++ b/Data/EmploymentSummary-2017.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18827"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1robb\PycharmProjects\Law_School\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7365"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="8520" tabRatio="186" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1337,7 +1337,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1664,11 +1664,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:FC224"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1677,6 +1677,135 @@
     <col min="2" max="2" width="32.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="32.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="35" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="27" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="29" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="36" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="36" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="64" max="65" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="69" max="70" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="7" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="74" max="75" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="79" max="80" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="84" max="85" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="89" max="90" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="94" max="95" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="99" max="100" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="104" max="105" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="109" max="110" width="21" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="112" max="112" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="17" bestFit="1" customWidth="1"/>
+    <col min="114" max="115" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="116" max="116" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="117" max="117" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="118" max="118" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="119" max="120" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="121" max="121" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="122" max="122" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="123" max="123" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="124" max="125" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="126" max="126" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="127" max="127" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="128" max="128" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="129" max="130" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="131" max="131" width="15" bestFit="1" customWidth="1"/>
+    <col min="132" max="132" width="10" bestFit="1" customWidth="1"/>
+    <col min="133" max="133" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="134" max="135" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="136" max="136" width="11" bestFit="1" customWidth="1"/>
+    <col min="137" max="137" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="138" max="138" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="139" max="140" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="141" max="141" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="142" max="142" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="143" max="143" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="144" max="145" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="146" max="146" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="147" max="147" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="148" max="148" width="10" bestFit="1" customWidth="1"/>
+    <col min="149" max="150" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="151" max="151" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="152" max="152" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="153" max="153" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="154" max="154" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="155" max="155" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="156" max="156" width="33" bestFit="1" customWidth="1"/>
+    <col min="157" max="157" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="158" max="158" width="31.140625" bestFit="1" customWidth="1"/>
     <col min="159" max="159" width="27.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>